<commit_message>
Acta de reunión del 16-09 y actualización de documentos involucrados
</commit_message>
<xml_diff>
--- a/docs/02 - Athos - Carpeta de Proyecto/Documentacion auxiliar/planilla de riesgos.xlsx
+++ b/docs/02 - Athos - Carpeta de Proyecto/Documentacion auxiliar/planilla de riesgos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31464540\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mis Documentos\ORT Analista de Sistemas\3° 2°\Integración de Sistemas\is\docs\02 - Athos - Carpeta de Proyecto\Documentacion auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DA1FBD-362B-4CEA-9E47-275842D095C4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="989"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -214,9 +215,6 @@
     <t>Error en la base de datos</t>
   </si>
   <si>
-    <t>Se realizaran copias de seguridad de la base de datos de manera regular</t>
-  </si>
-  <si>
     <t>Variable, puede suponer una catástrofe, o un simple retrabajo</t>
   </si>
   <si>
@@ -277,16 +275,19 @@
     <t>El paciente presiona el boton 'siguiente' mas de una vez y debido a un retraso en el refresco de la pantalla, ciertas preguntas son salteadas</t>
   </si>
   <si>
-    <t>Se saltean preguntas</t>
-  </si>
-  <si>
     <t>Se aplicara un retraso de medio segundo antes de habilitar los botones de respuesta</t>
+  </si>
+  <si>
+    <t>Se saltean preguntas involuntariamente</t>
+  </si>
+  <si>
+    <t>Se realizaran copias de seguridad de la base de datos local de manera regular a la nube</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -762,14 +763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F47" sqref="F47"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1028,7 +1029,7 @@
         <v>52</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>12</v>
@@ -1040,7 +1041,7 @@
         <v>53</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>55</v>
@@ -1066,7 +1067,7 @@
         <v>35</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>59</v>
@@ -1086,7 +1087,7 @@
         <v>61</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>21</v>
@@ -1095,13 +1096,13 @@
         <v>13</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>54</v>
@@ -1109,13 +1110,13 @@
     </row>
     <row r="11" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>42</v>
@@ -1124,13 +1125,13 @@
         <v>13</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>54</v>
@@ -1138,13 +1139,13 @@
     </row>
     <row r="12" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>12</v>
@@ -1156,7 +1157,7 @@
         <v>53</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>55</v>
@@ -1167,13 +1168,13 @@
     </row>
     <row r="13" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>12</v>
@@ -1185,7 +1186,7 @@
         <v>53</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>55</v>
@@ -1196,13 +1197,13 @@
     </row>
     <row r="14" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>42</v>
@@ -1211,7 +1212,7 @@
         <v>35</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Actualización de la planilla de riesgos
Se corrigieron algunos riesgos y se agregaron nuevos
</commit_message>
<xml_diff>
--- a/docs/02 - Athos - Carpeta de Proyecto/Documentacion auxiliar/planilla de riesgos.xlsx
+++ b/docs/02 - Athos - Carpeta de Proyecto/Documentacion auxiliar/planilla de riesgos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mis Documentos\ORT Analista de Sistemas\3° 2°\Integración de Sistemas\is\docs\02 - Athos - Carpeta de Proyecto\Documentacion auxiliar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcaba\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DA1FBD-362B-4CEA-9E47-275842D095C4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -188,9 +187,6 @@
     <t>Corte de luz</t>
   </si>
   <si>
-    <t>Guardar resultados parciales del test cada 10 minutos o 5 preguntas, dependiendo de lo que suceda primero</t>
-  </si>
-  <si>
     <t>Riesgo del producto</t>
   </si>
   <si>
@@ -224,9 +220,6 @@
     <t>El paciente se equivoca al cargar sus datos personales</t>
   </si>
   <si>
-    <t>Se le permitira al profesional editar los datos del paciente (previa solicitud del paciente)</t>
-  </si>
-  <si>
     <t>Puede derivar en un malentendido a la hora de querer asociar un diagnostico con un paciente</t>
   </si>
   <si>
@@ -239,18 +232,6 @@
     <t>Se corrompe la base de datos perdiéndose todos los registros</t>
   </si>
   <si>
-    <t>Diseño minimalista y permitir la edición del test cuando el protocolo del mismo permita</t>
-  </si>
-  <si>
-    <t>Se le solicita al paciente una confirmacion de los datos antes de empezar el test mediante una ventana de confirmación</t>
-  </si>
-  <si>
-    <t>Se retoma el test desde la última pregunta guardada</t>
-  </si>
-  <si>
-    <t>Se restaura la última copia de seguridad  que se realizo con éxito</t>
-  </si>
-  <si>
     <t>R11</t>
   </si>
   <si>
@@ -281,13 +262,117 @@
     <t>Se saltean preguntas involuntariamente</t>
   </si>
   <si>
-    <t>Se realizaran copias de seguridad de la base de datos local de manera regular a la nube</t>
+    <t>Rediseño de la interfaz visual.</t>
+  </si>
+  <si>
+    <t>Demora en la entrega final del producto o retrabajo.</t>
+  </si>
+  <si>
+    <t>Se realizan copias de seguridad de la base de datos de manera regular.</t>
+  </si>
+  <si>
+    <t>Se van guardando las respuestas en una tabla auxiliar a medida que se vayan respondiendo.</t>
+  </si>
+  <si>
+    <t>Se le solicita al paciente una confirmacion de los datos antes de empezar el test mediante una ventana de confirmación.</t>
+  </si>
+  <si>
+    <t>Se verifica con el cliente en todo momento que el diseño sea el adecuado.</t>
+  </si>
+  <si>
+    <t>Guardar cada respuesta en una tabla auxiliar.</t>
+  </si>
+  <si>
+    <t>Se retoma el test desde la última pregunta guardada, si corresponde.</t>
+  </si>
+  <si>
+    <t>Se restaura la última copia de seguridad  que se realizo con éxito.</t>
+  </si>
+  <si>
+    <t>Se le permitira al profesional editar los datos del paciente (previa solicitud del paciente).</t>
+  </si>
+  <si>
+    <t>Se retoma el test desde la última pregunta guardada.</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>La conexión entre la máquina donde se esta llevando a cabo el test y el servidos se ve interrumpida</t>
+  </si>
+  <si>
+    <t>Se llena la base de datos</t>
+  </si>
+  <si>
+    <t>Se interrumpe la conexión</t>
+  </si>
+  <si>
+    <t>La base de datos se queda sin espacio</t>
+  </si>
+  <si>
+    <t>Monitoreo de la base de datos y configuración de alertas.</t>
+  </si>
+  <si>
+    <t>Se agrega espacio a la base de datos.</t>
+  </si>
+  <si>
+    <t>Imposibilidad de tomar nuevos tests</t>
+  </si>
+  <si>
+    <t>Fallas en las copias de seguridad</t>
+  </si>
+  <si>
+    <t>Las copias de seguridad no se realizan exitosamente</t>
+  </si>
+  <si>
+    <t>* Se mantienen varias copias de seguridad
+* Notificaciones para saber como finalizaron las copias de respaldo
+* Cada cierto tiempo, se prueba reestablecer una de las copias de seguridad</t>
+  </si>
+  <si>
+    <t>Se investigan las causas de las fallas y se busca una solución.</t>
+  </si>
+  <si>
+    <t>Imposibilidad de recuperar la base de datos ante algún inconveniente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -763,27 +848,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="1"/>
     <col min="2" max="2" width="17" style="1"/>
-    <col min="3" max="3" width="24.85546875" style="1"/>
+    <col min="3" max="3" width="27" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="1"/>
     <col min="5" max="5" width="15.5703125" style="1"/>
     <col min="6" max="6" width="30.28515625" style="1"/>
-    <col min="7" max="7" width="33.7109375" style="1"/>
-    <col min="8" max="8" width="25.140625" style="1"/>
-    <col min="9" max="9" width="11.28515625" style="1"/>
+    <col min="7" max="7" width="37.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="1" customWidth="1"/>
     <col min="10" max="1025" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
@@ -816,7 +901,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:40" s="3" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:40" s="3" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -845,7 +930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:40" s="3" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:40" s="3" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -874,7 +959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:40" s="3" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:40" s="3" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
@@ -903,7 +988,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:40" s="3" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:40" s="3" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -932,7 +1017,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:40" s="3" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:40" s="3" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
@@ -961,7 +1046,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:40" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>46</v>
       </c>
@@ -1021,7 +1106,7 @@
       <c r="AM7" s="3"/>
       <c r="AN7" s="3"/>
     </row>
-    <row r="8" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>51</v>
       </c>
@@ -1029,7 +1114,7 @@
         <v>52</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>12</v>
@@ -1038,27 +1123,27 @@
         <v>35</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="5" t="s">
+    </row>
+    <row r="9" spans="1:40" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>12</v>
@@ -1067,27 +1152,27 @@
         <v>35</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="G9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="C10" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>21</v>
@@ -1096,27 +1181,27 @@
         <v>13</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="H10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>42</v>
@@ -1125,27 +1210,27 @@
         <v>13</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>12</v>
@@ -1154,27 +1239,27 @@
         <v>35</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="5" t="s">
+    </row>
+    <row r="13" spans="1:40" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>12</v>
@@ -1183,27 +1268,27 @@
         <v>35</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:40" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>42</v>
@@ -1212,16 +1297,164 @@
         <v>35</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I14" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>54</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Actualizacion de la planilla de gestion de riesgos
</commit_message>
<xml_diff>
--- a/docs/02 - Athos - Carpeta de Proyecto/Documentacion auxiliar/planilla de riesgos.xlsx
+++ b/docs/02 - Athos - Carpeta de Proyecto/Documentacion auxiliar/planilla de riesgos.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mis Documentos\ORT Analista de Sistemas\3° 2°\Integración de Sistemas\is\docs\02 - Athos - Carpeta de Proyecto\Documentacion auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C07333-B4FA-4370-9754-08BC46EF1016}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3018D8C-017A-496B-819F-A42013325516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10575" yWindow="3645" windowWidth="21600" windowHeight="11505" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="118">
   <si>
     <t>ID</t>
   </si>
@@ -376,6 +375,21 @@
   <si>
     <t>Se realiza una copia de emergencia replicada.
 Se investigan las causas de las fallas y se busca una solución a largo plazo.</t>
+  </si>
+  <si>
+    <t>Errores en el relevamiento por no poder interpretar el lenguaje del negocio</t>
+  </si>
+  <si>
+    <t>El lenguaje que utiliza el cliente en su negocio no es comprendido claramente por quien releva, generando confusiones</t>
+  </si>
+  <si>
+    <t>Se validan los documentos con el cliente y se intenta adoptar el lenguaje de su negocio en todo lo que respecta al proyecto</t>
+  </si>
+  <si>
+    <t>Se reelaboran los documentos con la supervisión y aprobación del cliente</t>
+  </si>
+  <si>
+    <t>Demora en los tiempos del proyecto y posible diseño erroneo</t>
   </si>
 </sst>
 </file>
@@ -400,7 +414,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,6 +443,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF73D216"/>
         <bgColor rgb="FF339966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -476,7 +496,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -864,10 +884,10 @@
   <dimension ref="A1:AMK37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1412,14 +1432,30 @@
       <c r="A18" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">

</xml_diff>

<commit_message>
Actualizacion de documentos de riesgo
</commit_message>
<xml_diff>
--- a/docs/02 - Athos - Carpeta de Proyecto/Documentacion auxiliar/planilla de riesgos.xlsx
+++ b/docs/02 - Athos - Carpeta de Proyecto/Documentacion auxiliar/planilla de riesgos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mis Documentos\ORT Analista de Sistemas\3° 2°\Integración de Sistemas\is\docs\02 - Athos - Carpeta de Proyecto\Documentacion auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3018D8C-017A-496B-819F-A42013325516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520E22BA-5C45-4834-89A7-3C0CB3DEC43B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34575" yWindow="1365" windowWidth="7305" windowHeight="9150" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -887,7 +887,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>